<commit_message>
soil weight file, worked on explore script
</commit_message>
<xml_diff>
--- a/Seedbank-Data/Soil_Weight.xlsx
+++ b/Seedbank-Data/Soil_Weight.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,6 +71,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -398,13 +403,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A81"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,404 +420,884 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2">
+        <v>1194.67</v>
+      </c>
+      <c r="C2">
+        <v>1213.1500000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3">
+        <v>1135.43</v>
+      </c>
+      <c r="C3">
+        <v>1083.57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="B4">
+        <v>1143.3900000000001</v>
+      </c>
+      <c r="C4">
+        <v>1116.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5">
+        <v>1100.47</v>
+      </c>
+      <c r="C5">
+        <v>1159.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6">
+        <v>1025.75</v>
+      </c>
+      <c r="C6">
+        <v>1087.9100000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B7">
+        <v>1155.3</v>
+      </c>
+      <c r="C7">
+        <v>1123.1600000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8">
+        <v>1076.75</v>
+      </c>
+      <c r="C8">
+        <v>1112.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="B9">
+        <v>1009.37</v>
+      </c>
+      <c r="C9">
+        <v>1113.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10">
+        <v>1035.55</v>
+      </c>
+      <c r="C10">
+        <v>1069.28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="B11">
+        <v>1181.45</v>
+      </c>
+      <c r="C11">
+        <v>1103.72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="B12">
+        <v>1190.58</v>
+      </c>
+      <c r="C12">
+        <v>1137.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="B13">
+        <v>1131.95</v>
+      </c>
+      <c r="C13">
+        <v>1100.3699999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="B14">
+        <v>1143.8800000000001</v>
+      </c>
+      <c r="C14">
+        <v>1124.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15">
+        <v>1128.99</v>
+      </c>
+      <c r="C15">
+        <v>1159.3900000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>901.15</v>
+      </c>
+      <c r="C16">
+        <v>962.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>1136.79</v>
+      </c>
+      <c r="C17">
+        <v>1153.6500000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>1103.08</v>
+      </c>
+      <c r="C18">
+        <v>1182.8900000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>1170.8399999999999</v>
+      </c>
+      <c r="C19">
+        <v>1139.96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>998.43</v>
+      </c>
+      <c r="C20">
+        <v>1050.8399999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>1096.5999999999999</v>
+      </c>
+      <c r="C21">
+        <v>1018.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>1125.8499999999999</v>
+      </c>
+      <c r="C22">
+        <v>1153.5899999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>1109.0899999999999</v>
+      </c>
+      <c r="C23">
+        <v>1153.9000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>1155.5899999999999</v>
+      </c>
+      <c r="C24">
+        <v>1110.1300000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>1098.75</v>
+      </c>
+      <c r="C25">
+        <v>1092.32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>1150.1300000000001</v>
+      </c>
+      <c r="C26">
+        <v>1166.0999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>1136.25</v>
+      </c>
+      <c r="C27">
+        <v>1188.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>1222.56</v>
+      </c>
+      <c r="C28">
+        <v>1235.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>1205.8499999999999</v>
+      </c>
+      <c r="C29">
+        <v>1207.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>1214.3399999999999</v>
+      </c>
+      <c r="C30">
+        <v>1120.6400000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>1250.99</v>
+      </c>
+      <c r="C31">
+        <v>1130.93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>1143.4100000000001</v>
+      </c>
+      <c r="C32">
+        <v>1030.8889999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>1081.5999999999999</v>
+      </c>
+      <c r="C33">
+        <v>1119.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34">
+        <v>1132.95</v>
+      </c>
+      <c r="C34">
+        <v>1174.33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35">
+        <v>855.1</v>
+      </c>
+      <c r="C35">
+        <v>879.65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36">
+        <v>1270.8399999999999</v>
+      </c>
+      <c r="C36">
+        <v>1287.45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37">
+        <v>1125.6500000000001</v>
+      </c>
+      <c r="C37">
+        <v>1174.69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38">
+        <v>1053.8499999999999</v>
+      </c>
+      <c r="C38">
+        <v>1067.71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39">
+        <v>1197.23</v>
+      </c>
+      <c r="C39">
+        <v>1133.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40">
+        <v>1139.42</v>
+      </c>
+      <c r="C40">
+        <v>1181.4000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41">
+        <v>1162.47</v>
+      </c>
+      <c r="C41">
+        <v>1036.22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42">
+        <v>1161.08</v>
+      </c>
+      <c r="C42">
+        <v>1197.32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43">
+        <v>1035.69</v>
+      </c>
+      <c r="C43">
+        <v>1093.97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44">
+        <v>904.37</v>
+      </c>
+      <c r="C44">
+        <v>979.41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45">
+        <v>976.51</v>
+      </c>
+      <c r="C45">
+        <v>1052.98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46">
+        <v>1141.06</v>
+      </c>
+      <c r="C46">
+        <v>1091.24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47">
+        <v>1125.3599999999999</v>
+      </c>
+      <c r="C47">
+        <v>1108.47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>1054.43</v>
+      </c>
+      <c r="C48">
+        <v>997.37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>1124.27</v>
+      </c>
+      <c r="C49">
+        <v>1195.9100000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>1050.69</v>
+      </c>
+      <c r="C50">
+        <v>1065.99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>1157.2</v>
+      </c>
+      <c r="C51">
+        <v>1135.68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>1137.8399999999999</v>
+      </c>
+      <c r="C52">
+        <v>1156.49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>1114.02</v>
+      </c>
+      <c r="C53">
+        <v>1081.8800000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>1174.68</v>
+      </c>
+      <c r="C54">
+        <v>1122.42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>1031.47</v>
+      </c>
+      <c r="C55">
+        <v>1013.51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>1182.46</v>
+      </c>
+      <c r="C56">
+        <v>1135.43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>1174.5899999999999</v>
+      </c>
+      <c r="C57">
+        <v>1100.3800000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>1115.0999999999999</v>
+      </c>
+      <c r="C58">
+        <v>1106.97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>883.31</v>
+      </c>
+      <c r="C59">
+        <v>896.93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60">
+        <v>1038.8499999999999</v>
+      </c>
+      <c r="C60">
+        <v>1086.27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61">
+        <v>1067.18</v>
+      </c>
+      <c r="C61">
+        <v>1044.8800000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62">
+        <v>1115.44</v>
+      </c>
+      <c r="C62">
+        <v>1067.99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>1193.31</v>
+      </c>
+      <c r="C63">
+        <v>1166.8699999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>1182.79</v>
+      </c>
+      <c r="C64">
+        <v>1146.03</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>980.68</v>
+      </c>
+      <c r="C65">
+        <v>1063.21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>887.19</v>
+      </c>
+      <c r="C66">
+        <v>887.38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>980.44</v>
+      </c>
+      <c r="C67">
+        <v>1003.63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>1182.3900000000001</v>
+      </c>
+      <c r="C68">
+        <v>1191.52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>1140.51</v>
+      </c>
+      <c r="C69">
+        <v>1154.9000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>963.31</v>
+      </c>
+      <c r="C70">
+        <v>926.85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>1058.5</v>
+      </c>
+      <c r="C71">
+        <v>1051.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>1124.8499999999999</v>
+      </c>
+      <c r="C72">
+        <v>1171.53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>819.72</v>
+      </c>
+      <c r="C73">
+        <v>814.31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>1123.95</v>
+      </c>
+      <c r="C74">
+        <v>1155.93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>1131.7</v>
+      </c>
+      <c r="C75">
+        <v>1161.08</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>1196</v>
+      </c>
+      <c r="C76">
+        <v>1140.75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>1167.25</v>
+      </c>
+      <c r="C77">
+        <v>1195.3399999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>1278.3699999999999</v>
+      </c>
+      <c r="C78">
+        <v>1215.28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>1243.97</v>
+      </c>
+      <c r="C79">
+        <v>1116.45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>1220.51</v>
+      </c>
+      <c r="C80">
+        <v>1237.6600000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
+      </c>
+      <c r="B81">
+        <v>1122.3399999999999</v>
+      </c>
+      <c r="C81">
+        <v>1122.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>